<commit_message>
outputs generated from model runs
</commit_message>
<xml_diff>
--- a/models/calculation engines/AL quarterly chart pack/Outputs/Data input annual Output.xlsx
+++ b/models/calculation engines/AL quarterly chart pack/Outputs/Data input annual Output.xlsx
@@ -1,37 +1,66 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Alumina Capacity</t>
+  </si>
+  <si>
+    <t>Alumina Production</t>
+  </si>
+  <si>
+    <t>Alumina Utilisation</t>
+  </si>
+  <si>
+    <t>Aluminium Capacity</t>
+  </si>
+  <si>
+    <t>Aluminium Production</t>
+  </si>
+  <si>
+    <t>Aluminium Utilisation</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,94 +75,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -421,586 +391,566 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Year</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Alumina Capacity</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Alumina Production</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Alumina Utilisation</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Aluminium Capacity</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Aluminium Production</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Aluminium Utilisation</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
         <v>2000</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>4.17</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>4.308157</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>1.033131175059952</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>3.50935</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>2.779375</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>0.7919913944177697</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:7">
+      <c r="A3">
         <v>2001</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>4.202</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>4.691664</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>1.116531175630652</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>4.22155</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>3.380251</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>0.8007132451350808</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:7">
+      <c r="A4">
         <v>2002</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>5.165</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>5.435734</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>1.052417037754114</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>5.35765</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>4.313508</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>0.8051119427360877</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:7">
+      <c r="A5">
         <v>2003</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>5.735</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5">
         <v>6.179648</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>1.077532345248474</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>7.39685</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5">
         <v>5.564244</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>0.7522450772964168</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:7">
+      <c r="A6">
         <v>2004</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>6.395</v>
       </c>
-      <c r="C6" t="n">
+      <c r="C6">
         <v>6.967852</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>1.089578107896794</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>8.80425</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>6.708283</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>0.7619369054717892</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:7">
+      <c r="A7">
         <v>2005</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>8.9</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7">
         <v>8.485488549999999</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>0.9534256797752808</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>9.7188</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7">
         <v>8.073785000000001</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>0.8307388772276414</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="8" spans="1:7">
+      <c r="A8">
         <v>2006</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>18.695</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8">
         <v>13.442813</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>0.7190592671837389</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>11.7251</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8">
         <v>9.658665363636359</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>0.8237597430841835</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row r="9" spans="1:7">
+      <c r="A9">
         <v>2007</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>27.295</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C9">
         <v>19.403</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>0.7108627953837698</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>15.3465</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9">
         <v>12.1733192889342</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>0.7932309835424494</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="10" spans="1:7">
+      <c r="A10">
         <v>2008</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>34.095</v>
       </c>
-      <c r="C10" t="n">
+      <c r="C10">
         <v>23.1633</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>0.679375274967004</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10">
         <v>16.7795</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10">
         <v>12.6804748829794</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>0.7557123205685152</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row r="11" spans="1:7">
+      <c r="A11">
         <v>2009</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>36.195</v>
       </c>
-      <c r="C11" t="n">
+      <c r="C11">
         <v>24.5850825688073</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>0.6792397449594503</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>20.0145</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11">
         <v>12.7033315838769</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>0.6347064170414898</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
+    <row r="12" spans="1:7">
+      <c r="A12">
         <v>2010</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>43.165</v>
       </c>
-      <c r="C12" t="n">
+      <c r="C12">
         <v>29.3446751041467</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>0.6798256713575049</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>22.4855</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12">
         <v>15.5488568118829</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12">
         <v>0.6915059399116276</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
+    <row r="13" spans="1:7">
+      <c r="A13">
         <v>2011</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>51.495</v>
       </c>
-      <c r="C13" t="n">
+      <c r="C13">
         <v>33.7011546579369</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>0.6544548918911913</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>24.798</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13">
         <v>17.3453646386334</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13">
         <v>0.6994662730314299</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="n">
+    <row r="14" spans="1:7">
+      <c r="A14">
         <v>2012</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>59.69</v>
       </c>
-      <c r="C14" t="n">
+      <c r="C14">
         <v>40.986</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>0.6866476796783381</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>30.35</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14">
         <v>22.7196995969173</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14">
         <v>0.7485897725508172</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="n">
+    <row r="15" spans="1:7">
+      <c r="A15">
         <v>2013</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>64.12</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C15">
         <v>48.065</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>0.749610106051154</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>36.75</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15">
         <v>24.5809559838411</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15">
         <v>0.6688695505807102</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="n">
+    <row r="16" spans="1:7">
+      <c r="A16">
         <v>2014</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>68.31999999999999</v>
       </c>
-      <c r="C16" t="n">
+      <c r="C16">
         <v>50.658</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>0.7414812646370025</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>39.5</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16">
         <v>26.5442497897503</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16">
         <v>0.6720063237911468</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="n">
+    <row r="17" spans="1:7">
+      <c r="A17">
         <v>2015</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>73.37</v>
       </c>
-      <c r="C17" t="n">
+      <c r="C17">
         <v>56.163</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17">
         <v>0.7654763527327244</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>41.7</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17">
         <v>30.693</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17">
         <v>0.7360431654676259</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="n">
+    <row r="18" spans="1:7">
+      <c r="A18">
         <v>2016</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>76.56999999999999</v>
       </c>
-      <c r="C18" t="n">
+      <c r="C18">
         <v>60.898</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18">
         <v>0.7953245396369336</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18">
         <v>44.859</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18">
         <v>32.465</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18">
         <v>0.7237120756147039</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="n">
+    <row r="19" spans="1:7">
+      <c r="A19">
         <v>2017</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>82.59999999999999</v>
       </c>
-      <c r="C19" t="n">
+      <c r="C19">
         <v>69.02</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19">
         <v>0.8355932203389831</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19">
         <v>46.932</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19">
         <v>36.6</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19">
         <v>0.7798517003323958</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="n">
+    <row r="20" spans="1:7">
+      <c r="A20">
         <v>2018</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>86.2</v>
       </c>
-      <c r="C20" t="n">
+      <c r="C20">
         <v>70.8</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20">
         <v>0.8213457076566125</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20">
         <v>45.955</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20">
         <v>36.3</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20">
         <v>0.7899031661407899</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="n">
+    <row r="21" spans="1:7">
+      <c r="A21">
         <v>2019</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>88.81999999999999</v>
       </c>
-      <c r="C21" t="n">
+      <c r="C21">
         <v>70.81</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21">
         <v>0.7972303535239812</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21">
         <v>43.9</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21">
         <v>35.5</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21">
         <v>0.8086560364464693</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="n">
+    <row r="22" spans="1:7">
+      <c r="A22">
         <v>2020</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>92.81999999999999</v>
       </c>
-      <c r="C22" t="n">
+      <c r="C22">
         <v>73.5</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22">
         <v>0.7918552036199096</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22">
         <v>44.35</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22">
         <v>36.8</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G22">
         <v>0.8297632468996617</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="n">
+    <row r="23" spans="1:7">
+      <c r="A23">
         <v>2021</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>96.22</v>
       </c>
-      <c r="C23" t="n">
+      <c r="C23">
         <v>76.90000000000001</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23">
         <v>0.7992101434213262</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23">
         <v>44.8</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23">
         <v>38.2</v>
       </c>
-      <c r="G23" t="n">
+      <c r="G23">
         <v>0.8526785714285715</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="n">
+    <row r="24" spans="1:7">
+      <c r="A24">
         <v>2022</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>100.32</v>
       </c>
-      <c r="C24" t="n">
+      <c r="C24">
         <v>79.3</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24">
         <v>0.7904704944178629</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24">
         <v>45.1</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24">
         <v>39</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G24">
         <v>0.8647450110864745</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>